<commit_message>
ADD some results for Abschlussveranstaltung
</commit_message>
<xml_diff>
--- a/inst/extdata/Data_entry/Abschlussveranstaltung.xlsx
+++ b/inst/extdata/Data_entry/Abschlussveranstaltung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amatzi\Documents\github-repos\r2q\inst\extdata\Data_entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86881689-7F86-4051-9225-D4B9C54B024E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B97FED-CB0F-449D-B8ED-AF4896E2FA14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="108" windowWidth="28524" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1191,7 +1191,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="30">
-        <v>1.26</v>
+        <v>0.85</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
All new, all better
</commit_message>
<xml_diff>
--- a/inst/extdata/Data_entry/Abschlussveranstaltung.xlsx
+++ b/inst/extdata/Data_entry/Abschlussveranstaltung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20387"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amatzi\Documents\github-repos\r2q\inst\extdata\Data_entry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\r2q\inst\extdata\Data_entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B97FED-CB0F-449D-B8ED-AF4896E2FA14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04516C3A-6454-460B-A533-021B75A6A541}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="28524" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="110" windowWidth="19080" windowHeight="6820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_data" sheetId="1" r:id="rId1"/>
@@ -19,24 +19,18 @@
     <sheet name="pollution_data" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="area_plan">site_data!$C$15</definedName>
+    <definedName name="area_plan">site_data!$D$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="90">
-  <si>
-    <t>Parameter</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="120">
   <si>
     <t>Value</t>
   </si>
   <si>
-    <t>Explanation</t>
-  </si>
-  <si>
     <t>SUW_name</t>
   </si>
   <si>
@@ -94,18 +88,9 @@
     <t>annual rainfall [mm/yr]</t>
   </si>
   <si>
-    <t>l/(s*kmì)</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>area_plan</t>
   </si>
   <si>
-    <t>Obligatory</t>
-  </si>
-  <si>
     <t>Natural run-off of urban area ("area_catch") for a yearly rain event</t>
   </si>
   <si>
@@ -296,6 +281,111 @@
   </si>
   <si>
     <t>urbanised area further upstream that is not considered in "area_urban"</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>l/(s*km2)</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>f_id</t>
+  </si>
+  <si>
+    <t>primary_function</t>
+  </si>
+  <si>
+    <t>characaterisation 1</t>
+  </si>
+  <si>
+    <t>characaterisation 2</t>
+  </si>
+  <si>
+    <t>characaterisation 3</t>
+  </si>
+  <si>
+    <t>Residential Building</t>
+  </si>
+  <si>
+    <t>Commercial/industrial Building</t>
+  </si>
+  <si>
+    <t>Yard</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>High traffic</t>
+  </si>
+  <si>
+    <t>Medium traffic</t>
+  </si>
+  <si>
+    <t>low traffic</t>
+  </si>
+  <si>
+    <t>very low traffic</t>
+  </si>
+  <si>
+    <t>In high traffic area</t>
+  </si>
+  <si>
+    <t>In low traffic area</t>
+  </si>
+  <si>
+    <t>Zinc roof</t>
+  </si>
+  <si>
+    <t>Green roof</t>
+  </si>
+  <si>
+    <t>Bitumen roof</t>
+  </si>
+  <si>
+    <t>Tiles, glas, other metal roof</t>
+  </si>
+  <si>
+    <t>Wihtout gaps</t>
+  </si>
+  <si>
+    <t>Open gaps</t>
+  </si>
+  <si>
+    <t>With biocides / unknown</t>
+  </si>
+  <si>
+    <t>Without biocides</t>
+  </si>
+  <si>
+    <t>area_m2</t>
+  </si>
+  <si>
+    <t>pah</t>
+  </si>
+  <si>
+    <t>nutrients</t>
+  </si>
+  <si>
+    <t>biocides</t>
+  </si>
+  <si>
+    <t>suspended_solids</t>
+  </si>
+  <si>
+    <t>Treatment in % (either average removal or area with complete removal)</t>
+  </si>
+  <si>
+    <t>heavy metals</t>
+  </si>
+  <si>
+    <t>phthalate</t>
   </si>
 </sst>
 </file>
@@ -340,7 +430,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,8 +479,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -533,28 +635,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -572,7 +652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -630,22 +710,18 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -663,6 +739,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -971,330 +1053,346 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.21875" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="62" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="62" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>33</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="F1" s="24"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="43" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="7">
+        <v>19</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7">
+      <c r="D5" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.54</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="7">
+        <v>5000</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="7">
+        <v>822</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="7">
-        <v>0.04</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="7">
-        <v>0.54</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="7">
-        <v>5000</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="7">
-        <v>822</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="46" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B9" s="47"/>
       <c r="C9" s="47"/>
-      <c r="D9" s="48"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="38" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>66</v>
       </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>61</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30">
         <v>3813634.44</v>
       </c>
-      <c r="D11" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="E11" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30">
+        <v>2753912.5</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="8">
+        <v>5.2</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="30">
+        <v>0.85</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="30">
+        <v>2.4E-2</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="30">
+        <v>0</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="39">
+        <v>16</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="E19" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="30">
-        <v>2753912.5</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="8">
-        <v>5.2</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="30">
-        <v>0.85</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="30">
-        <v>2.4E-2</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="30">
-        <v>0</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="41">
-        <v>0.1</v>
-      </c>
-      <c r="D19" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="3"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="2"/>
-      <c r="D20"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E21" s="3"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="E20"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D22"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1305,35 +1403,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289A40E2-2E80-40B7-B15A-A7ACC55EFECA}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B2" s="26">
         <v>0.75</v>
@@ -1345,9 +1443,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B3" s="26">
         <v>0.71</v>
@@ -1359,9 +1457,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B4" s="26">
         <v>0.73</v>
@@ -1373,9 +1471,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B5" s="26">
         <v>0.94</v>
@@ -1387,9 +1485,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B6" s="34">
         <v>0</v>
@@ -1406,14 +1504,1462 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE5508C-700E-4B9F-9966-495F6EFAF069}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:BA137"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="8" max="12" width="15.6328125" customWidth="1"/>
+    <col min="13" max="53" width="10.90625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="42"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="M2" s="41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="26">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26">
+        <v>1</v>
+      </c>
+      <c r="G3" s="40">
+        <v>0</v>
+      </c>
+      <c r="H3" s="40">
+        <v>0</v>
+      </c>
+      <c r="I3" s="40">
+        <v>0</v>
+      </c>
+      <c r="J3" s="40">
+        <v>0</v>
+      </c>
+      <c r="K3" s="40">
+        <v>0</v>
+      </c>
+      <c r="L3" s="40">
+        <v>0</v>
+      </c>
+      <c r="M3" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="26">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="40">
+        <v>7800</v>
+      </c>
+      <c r="H4" s="40">
+        <v>0</v>
+      </c>
+      <c r="I4" s="40">
+        <v>0</v>
+      </c>
+      <c r="J4" s="40">
+        <v>0</v>
+      </c>
+      <c r="K4" s="40">
+        <v>0</v>
+      </c>
+      <c r="L4" s="40">
+        <v>0</v>
+      </c>
+      <c r="M4" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="26">
+        <v>3</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="40">
+        <v>0</v>
+      </c>
+      <c r="H5" s="40">
+        <v>0</v>
+      </c>
+      <c r="I5" s="40">
+        <v>0</v>
+      </c>
+      <c r="J5" s="40">
+        <v>0</v>
+      </c>
+      <c r="K5" s="40">
+        <v>0</v>
+      </c>
+      <c r="L5" s="40">
+        <v>0</v>
+      </c>
+      <c r="M5" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="26">
+        <v>4</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G6" s="40">
+        <v>0</v>
+      </c>
+      <c r="H6" s="40">
+        <v>0</v>
+      </c>
+      <c r="I6" s="40">
+        <v>0</v>
+      </c>
+      <c r="J6" s="40">
+        <v>0</v>
+      </c>
+      <c r="K6" s="40">
+        <v>0</v>
+      </c>
+      <c r="L6" s="40">
+        <v>0</v>
+      </c>
+      <c r="M6" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="26">
+        <v>5</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G7" s="40">
+        <v>0</v>
+      </c>
+      <c r="H7" s="40">
+        <v>0</v>
+      </c>
+      <c r="I7" s="40">
+        <v>0</v>
+      </c>
+      <c r="J7" s="40">
+        <v>0</v>
+      </c>
+      <c r="K7" s="40">
+        <v>0</v>
+      </c>
+      <c r="L7" s="40">
+        <v>0</v>
+      </c>
+      <c r="M7" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="26">
+        <v>6</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26">
+        <v>1</v>
+      </c>
+      <c r="G8" s="40">
+        <v>0</v>
+      </c>
+      <c r="H8" s="40">
+        <v>0</v>
+      </c>
+      <c r="I8" s="40">
+        <v>0</v>
+      </c>
+      <c r="J8" s="40">
+        <v>0</v>
+      </c>
+      <c r="K8" s="40">
+        <v>0</v>
+      </c>
+      <c r="L8" s="40">
+        <v>0</v>
+      </c>
+      <c r="M8" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="26">
+        <v>7</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26">
+        <v>1</v>
+      </c>
+      <c r="G9" s="40">
+        <v>0</v>
+      </c>
+      <c r="H9" s="40">
+        <v>0</v>
+      </c>
+      <c r="I9" s="40">
+        <v>0</v>
+      </c>
+      <c r="J9" s="40">
+        <v>0</v>
+      </c>
+      <c r="K9" s="40">
+        <v>0</v>
+      </c>
+      <c r="L9" s="40">
+        <v>0</v>
+      </c>
+      <c r="M9" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="26">
+        <v>8</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="40">
+        <v>0</v>
+      </c>
+      <c r="H10" s="40">
+        <v>0</v>
+      </c>
+      <c r="I10" s="40">
+        <v>0</v>
+      </c>
+      <c r="J10" s="40">
+        <v>0</v>
+      </c>
+      <c r="K10" s="40">
+        <v>0</v>
+      </c>
+      <c r="L10" s="40">
+        <v>0</v>
+      </c>
+      <c r="M10" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="26">
+        <v>9</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="40">
+        <v>0</v>
+      </c>
+      <c r="H11" s="40">
+        <v>0</v>
+      </c>
+      <c r="I11" s="40">
+        <v>0</v>
+      </c>
+      <c r="J11" s="40">
+        <v>0</v>
+      </c>
+      <c r="K11" s="40">
+        <v>0</v>
+      </c>
+      <c r="L11" s="40">
+        <v>0</v>
+      </c>
+      <c r="M11" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="26">
+        <v>10</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G12" s="40">
+        <v>0</v>
+      </c>
+      <c r="H12" s="40">
+        <v>0</v>
+      </c>
+      <c r="I12" s="40">
+        <v>0</v>
+      </c>
+      <c r="J12" s="40">
+        <v>0</v>
+      </c>
+      <c r="K12" s="40">
+        <v>0</v>
+      </c>
+      <c r="L12" s="40">
+        <v>0</v>
+      </c>
+      <c r="M12" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="26">
+        <v>11</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G13" s="40">
+        <v>0</v>
+      </c>
+      <c r="H13" s="40">
+        <v>0</v>
+      </c>
+      <c r="I13" s="40">
+        <v>0</v>
+      </c>
+      <c r="J13" s="40">
+        <v>0</v>
+      </c>
+      <c r="K13" s="40">
+        <v>0</v>
+      </c>
+      <c r="L13" s="40">
+        <v>0</v>
+      </c>
+      <c r="M13" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="26">
+        <v>12</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26">
+        <v>1</v>
+      </c>
+      <c r="G14" s="40">
+        <v>0</v>
+      </c>
+      <c r="H14" s="40">
+        <v>0</v>
+      </c>
+      <c r="I14" s="40">
+        <v>0</v>
+      </c>
+      <c r="J14" s="40">
+        <v>0</v>
+      </c>
+      <c r="K14" s="40">
+        <v>0</v>
+      </c>
+      <c r="L14" s="40">
+        <v>0</v>
+      </c>
+      <c r="M14" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="26">
+        <v>13</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26">
+        <v>1</v>
+      </c>
+      <c r="G15" s="40">
+        <v>0</v>
+      </c>
+      <c r="H15" s="40">
+        <v>0</v>
+      </c>
+      <c r="I15" s="40">
+        <v>0</v>
+      </c>
+      <c r="J15" s="40">
+        <v>0</v>
+      </c>
+      <c r="K15" s="40">
+        <v>0</v>
+      </c>
+      <c r="L15" s="40">
+        <v>0</v>
+      </c>
+      <c r="M15" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="26">
+        <v>14</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="40">
+        <v>0</v>
+      </c>
+      <c r="H16" s="40">
+        <v>0</v>
+      </c>
+      <c r="I16" s="40">
+        <v>0</v>
+      </c>
+      <c r="J16" s="40">
+        <v>0</v>
+      </c>
+      <c r="K16" s="40">
+        <v>0</v>
+      </c>
+      <c r="L16" s="40">
+        <v>0</v>
+      </c>
+      <c r="M16" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="26">
+        <v>15</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="40">
+        <v>0</v>
+      </c>
+      <c r="H17" s="40">
+        <v>0</v>
+      </c>
+      <c r="I17" s="40">
+        <v>0</v>
+      </c>
+      <c r="J17" s="40">
+        <v>0</v>
+      </c>
+      <c r="K17" s="40">
+        <v>0</v>
+      </c>
+      <c r="L17" s="40">
+        <v>0</v>
+      </c>
+      <c r="M17" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="26">
+        <v>16</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G18" s="40">
+        <v>0</v>
+      </c>
+      <c r="H18" s="40">
+        <v>0</v>
+      </c>
+      <c r="I18" s="40">
+        <v>0</v>
+      </c>
+      <c r="J18" s="40">
+        <v>0</v>
+      </c>
+      <c r="K18" s="40">
+        <v>0</v>
+      </c>
+      <c r="L18" s="40">
+        <v>0</v>
+      </c>
+      <c r="M18" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="26">
+        <v>17</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F19" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G19" s="40">
+        <v>0</v>
+      </c>
+      <c r="H19" s="40">
+        <v>0</v>
+      </c>
+      <c r="I19" s="40">
+        <v>0</v>
+      </c>
+      <c r="J19" s="40">
+        <v>0</v>
+      </c>
+      <c r="K19" s="40">
+        <v>0</v>
+      </c>
+      <c r="L19" s="40">
+        <v>0</v>
+      </c>
+      <c r="M19" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="26">
+        <v>18</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26">
+        <v>1</v>
+      </c>
+      <c r="G20" s="40">
+        <v>0</v>
+      </c>
+      <c r="H20" s="40">
+        <v>0</v>
+      </c>
+      <c r="I20" s="40">
+        <v>0</v>
+      </c>
+      <c r="J20" s="40">
+        <v>0</v>
+      </c>
+      <c r="K20" s="40">
+        <v>0</v>
+      </c>
+      <c r="L20" s="40">
+        <v>0</v>
+      </c>
+      <c r="M20" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="26">
+        <v>19</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26">
+        <v>1</v>
+      </c>
+      <c r="G21" s="40">
+        <v>0</v>
+      </c>
+      <c r="H21" s="40">
+        <v>0</v>
+      </c>
+      <c r="I21" s="40">
+        <v>0</v>
+      </c>
+      <c r="J21" s="40">
+        <v>0</v>
+      </c>
+      <c r="K21" s="40">
+        <v>0</v>
+      </c>
+      <c r="L21" s="40">
+        <v>0</v>
+      </c>
+      <c r="M21" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="26">
+        <v>20</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="G22" s="40">
+        <v>0</v>
+      </c>
+      <c r="H22" s="40">
+        <v>0</v>
+      </c>
+      <c r="I22" s="40">
+        <v>0</v>
+      </c>
+      <c r="J22" s="40">
+        <v>0</v>
+      </c>
+      <c r="K22" s="40">
+        <v>0</v>
+      </c>
+      <c r="L22" s="40">
+        <v>0</v>
+      </c>
+      <c r="M22" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="26">
+        <v>21</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="40">
+        <v>0</v>
+      </c>
+      <c r="H23" s="40">
+        <v>0</v>
+      </c>
+      <c r="I23" s="40">
+        <v>0</v>
+      </c>
+      <c r="J23" s="40">
+        <v>0</v>
+      </c>
+      <c r="K23" s="40">
+        <v>0</v>
+      </c>
+      <c r="L23" s="40">
+        <v>0</v>
+      </c>
+      <c r="M23" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="26">
+        <v>22</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G24" s="40">
+        <v>0</v>
+      </c>
+      <c r="H24" s="40">
+        <v>0</v>
+      </c>
+      <c r="I24" s="40">
+        <v>0</v>
+      </c>
+      <c r="J24" s="40">
+        <v>0</v>
+      </c>
+      <c r="K24" s="40">
+        <v>0</v>
+      </c>
+      <c r="L24" s="40">
+        <v>0</v>
+      </c>
+      <c r="M24" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="26">
+        <v>23</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G25" s="40">
+        <v>0</v>
+      </c>
+      <c r="H25" s="40">
+        <v>0</v>
+      </c>
+      <c r="I25" s="40">
+        <v>0</v>
+      </c>
+      <c r="J25" s="40">
+        <v>0</v>
+      </c>
+      <c r="K25" s="40">
+        <v>0</v>
+      </c>
+      <c r="L25" s="40">
+        <v>0</v>
+      </c>
+      <c r="M25" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="26">
+        <v>24</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26">
+        <v>1</v>
+      </c>
+      <c r="G26" s="40">
+        <v>0</v>
+      </c>
+      <c r="H26" s="40">
+        <v>0</v>
+      </c>
+      <c r="I26" s="40">
+        <v>0</v>
+      </c>
+      <c r="J26" s="40">
+        <v>0</v>
+      </c>
+      <c r="K26" s="40">
+        <v>0</v>
+      </c>
+      <c r="L26" s="40">
+        <v>0</v>
+      </c>
+      <c r="M26" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="26">
+        <v>25</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G27" s="40">
+        <v>0</v>
+      </c>
+      <c r="H27" s="40">
+        <v>0</v>
+      </c>
+      <c r="I27" s="40">
+        <v>0</v>
+      </c>
+      <c r="J27" s="40">
+        <v>0</v>
+      </c>
+      <c r="K27" s="40">
+        <v>0</v>
+      </c>
+      <c r="L27" s="40">
+        <v>0</v>
+      </c>
+      <c r="M27" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="26">
+        <v>26</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="40">
+        <v>0</v>
+      </c>
+      <c r="H28" s="40">
+        <v>0</v>
+      </c>
+      <c r="I28" s="40">
+        <v>0</v>
+      </c>
+      <c r="J28" s="40">
+        <v>0</v>
+      </c>
+      <c r="K28" s="40">
+        <v>0</v>
+      </c>
+      <c r="L28" s="40">
+        <v>0</v>
+      </c>
+      <c r="M28" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="26">
+        <v>27</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G29" s="40">
+        <v>0</v>
+      </c>
+      <c r="H29" s="40">
+        <v>0</v>
+      </c>
+      <c r="I29" s="40">
+        <v>0</v>
+      </c>
+      <c r="J29" s="40">
+        <v>0</v>
+      </c>
+      <c r="K29" s="40">
+        <v>0</v>
+      </c>
+      <c r="L29" s="40">
+        <v>0</v>
+      </c>
+      <c r="M29" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="26">
+        <v>28</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="40">
+        <v>0</v>
+      </c>
+      <c r="H30" s="40">
+        <v>0</v>
+      </c>
+      <c r="I30" s="40">
+        <v>0</v>
+      </c>
+      <c r="J30" s="40">
+        <v>0</v>
+      </c>
+      <c r="K30" s="40">
+        <v>0</v>
+      </c>
+      <c r="L30" s="40">
+        <v>0</v>
+      </c>
+      <c r="M30" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="26">
+        <v>29</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G31" s="40">
+        <v>0</v>
+      </c>
+      <c r="H31" s="40">
+        <v>0</v>
+      </c>
+      <c r="I31" s="40">
+        <v>0</v>
+      </c>
+      <c r="J31" s="40">
+        <v>0</v>
+      </c>
+      <c r="K31" s="40">
+        <v>0</v>
+      </c>
+      <c r="L31" s="40">
+        <v>0</v>
+      </c>
+      <c r="M31" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" s="26">
+        <v>30</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G32" s="40">
+        <v>0</v>
+      </c>
+      <c r="H32" s="40">
+        <v>0</v>
+      </c>
+      <c r="I32" s="40">
+        <v>0</v>
+      </c>
+      <c r="J32" s="40">
+        <v>0</v>
+      </c>
+      <c r="K32" s="40">
+        <v>0</v>
+      </c>
+      <c r="L32" s="40">
+        <v>0</v>
+      </c>
+      <c r="M32" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33" s="26">
+        <v>31</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G33" s="40">
+        <v>0</v>
+      </c>
+      <c r="H33" s="40">
+        <v>0</v>
+      </c>
+      <c r="I33" s="40">
+        <v>0</v>
+      </c>
+      <c r="J33" s="40">
+        <v>0</v>
+      </c>
+      <c r="K33" s="40">
+        <v>0</v>
+      </c>
+      <c r="L33" s="40">
+        <v>0</v>
+      </c>
+      <c r="M33" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34" s="26">
+        <v>32</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G34" s="40">
+        <v>0</v>
+      </c>
+      <c r="H34" s="40">
+        <v>0</v>
+      </c>
+      <c r="I34" s="40">
+        <v>0</v>
+      </c>
+      <c r="J34" s="40">
+        <v>0</v>
+      </c>
+      <c r="K34" s="40">
+        <v>0</v>
+      </c>
+      <c r="L34" s="40">
+        <v>0</v>
+      </c>
+      <c r="M34" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="49" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="50" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="51" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="52" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="53" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="54" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="55" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="56" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="57" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="58" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="59" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="60" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="61" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="62" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="63" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="64" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="65" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="66" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="67" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="68" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="69" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="70" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="71" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="72" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="73" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="74" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="75" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="76" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="77" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="78" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="79" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="80" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="81" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="82" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="83" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="84" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="85" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="86" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="87" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="88" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="89" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="90" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="91" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="92" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="93" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="94" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="95" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="96" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="97" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="98" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="99" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="100" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="101" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="102" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="103" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="104" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="105" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="106" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="107" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="108" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="109" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="110" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="111" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="112" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="113" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="114" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="115" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="116" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="117" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="118" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="119" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="120" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="121" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="122" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="123" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="124" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="125" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="126" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="127" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="128" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="129" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="130" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="131" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="132" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="133" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="134" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="135" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="136" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="137" s="42" customFormat="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:M1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1426,320 +2972,320 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="22">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="22">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C3" s="22">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="B6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C7" s="22">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>42</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C9" s="22">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C10" s="22">
         <v>0.186</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C11" s="22">
         <v>1.6E-2</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
-        <v>52</v>
-      </c>
       <c r="B12" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C12" s="22">
         <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C13" s="22">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C14" s="22">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C15" s="22">
         <v>2E-3</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C16" s="22">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>42</v>
-      </c>
       <c r="D17" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C18" s="22">
         <v>4.742</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C19" s="22">
         <v>2.1920000000000002</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C21" s="22">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C22" s="23">
         <v>0.108</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>